<commit_message>
More of the tables
</commit_message>
<xml_diff>
--- a/Arealtabeller hav forslag_v2.xlsx
+++ b/Arealtabeller hav forslag_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au207185\Dropbox\Projekt\SustainScapes\Biodiversitetsrådet DATA\Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Nat_BDR-data\Arealanalyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>Omfang af beskyttede områder</t>
   </si>
@@ -177,12 +177,6 @@
     <t>Men hvad er muligt</t>
   </si>
   <si>
-    <t>+anden beskyt.</t>
-  </si>
-  <si>
-    <t>Kun Nat.2000</t>
-  </si>
-  <si>
     <t>Samlet</t>
   </si>
   <si>
@@ -211,6 +205,15 @@
   </si>
   <si>
     <t>Ramsar</t>
+  </si>
+  <si>
+    <t>overlappet</t>
+  </si>
+  <si>
+    <t>area km2</t>
+  </si>
+  <si>
+    <t>% of Natura 2000</t>
   </si>
 </sst>
 </file>
@@ -830,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,7 +927,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>12</v>
@@ -939,7 +942,7 @@
       <c r="C10" s="13"/>
       <c r="G10" s="14"/>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -954,7 +957,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>15</v>
@@ -1011,7 +1014,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="F17"/>
       <c r="K17" s="14"/>
@@ -1089,7 +1092,7 @@
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="26" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1164,28 +1167,28 @@
       <c r="C32" s="27"/>
       <c r="N32" s="14"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B33" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="27"/>
       <c r="N33" s="14"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="27"/>
       <c r="N34" s="14"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B35" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="27"/>
       <c r="N35" s="14"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B36" s="16" t="s">
         <v>14</v>
       </c>
@@ -1202,59 +1205,62 @@
       <c r="M36" s="28"/>
       <c r="N36" s="29"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B37" s="19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B41" s="31" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="25" t="s">
+      <c r="D42" s="33"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B43" s="15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B42" s="8" t="s">
+      <c r="D43" s="33"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="33"/>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B43" s="15" t="s">
+      <c r="D44" s="33"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B45" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="33"/>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B44" s="15" t="s">
+      <c r="D45" s="33"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B46" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="33"/>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B45" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="33"/>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B46" s="34" t="s">
-        <v>49</v>
-      </c>
       <c r="D46" s="33"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B47" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D47" s="33"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B48" s="38" t="s">
         <v>9</v>
       </c>
@@ -1400,12 +1406,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1541,15 +1544,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CB331F7-BBA2-4EB0-A7A9-6210A4AB215D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{766D1400-9080-45E0-A13F-41B3A65F8D73}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2c0adeb0-4d61-4543-a46c-962a15d7310c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1573,17 +1587,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{766D1400-9080-45E0-A13F-41B3A65F8D73}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CB331F7-BBA2-4EB0-A7A9-6210A4AB215D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2c0adeb0-4d61-4543-a46c-962a15d7310c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>